<commit_message>
add missing df to these tables
</commit_message>
<xml_diff>
--- a/tables/Appendix Table S3_+Spores_TP_SEM_output.xlsx
+++ b/tables/Appendix Table S3_+Spores_TP_SEM_output.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/mlfearon_umich_edu/Documents/PROJECTS/Rachel Bag Experiment SEM/Data and Code/nutrient-bag-expt/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/mlfearon_umich_edu/Documents/PROJECTS/Manuscripts/Parasitism alters effects of mixing and nutrients - Oecologia/Data and Code/nutrient-bag-expt/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="13_ncr:1_{30DD4396-0B1C-4FB5-8F80-5AF9AEBFCAB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA36073A-54EB-40BA-90FF-6FB4445F6B95}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="13_ncr:1_{30DD4396-0B1C-4FB5-8F80-5AF9AEBFCAB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{977861CB-9BC1-4245-AFA6-0622027781F5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{45B3C3C3-E525-4F33-8866-CCD620B1EB35}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="16920" windowHeight="10540" xr2:uid="{45B3C3C3-E525-4F33-8866-CCD620B1EB35}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -308,10 +308,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -614,20 +610,20 @@
   <dimension ref="B2:M19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.81640625" customWidth="1"/>
+    <col min="3" max="3" width="19.26953125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:13" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="2:13" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -657,7 +653,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
@@ -689,7 +685,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B5" s="9" t="s">
         <v>15</v>
       </c>
@@ -717,7 +713,7 @@
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B6" s="16" t="s">
         <v>15</v>
       </c>
@@ -733,7 +729,9 @@
       <c r="F6" s="14">
         <v>6.2842243623436296E-3</v>
       </c>
-      <c r="G6" s="6"/>
+      <c r="G6" s="6">
+        <v>79</v>
+      </c>
       <c r="H6" s="14">
         <v>-1.62195983393488</v>
       </c>
@@ -743,7 +741,7 @@
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B7" s="9" t="s">
         <v>11</v>
       </c>
@@ -772,7 +770,7 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B8" s="6" t="s">
         <v>11</v>
       </c>
@@ -800,7 +798,7 @@
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B9" s="7" t="s">
         <v>18</v>
       </c>
@@ -832,7 +830,7 @@
         <v>0.73</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B10" s="6" t="s">
         <v>18</v>
       </c>
@@ -860,7 +858,7 @@
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
     </row>
-    <row r="11" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="8" t="s">
         <v>11</v>
       </c>
@@ -889,16 +887,16 @@
       <c r="K11" s="10"/>
       <c r="M11" s="9"/>
     </row>
-    <row r="12" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:13" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="17" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
     </row>
-    <row r="18" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
     </row>
-    <row r="19" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="7:8" x14ac:dyDescent="0.35">
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
     </row>

</xml_diff>